<commit_message>
update latest fix in bot and timesheet.py
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -895,13 +895,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -909,7 +909,11 @@
       <c r="G20" t="n">
         <v>0</v>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">

</xml_diff>

<commit_message>
fix the sampel calender flow
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -635,14 +635,14 @@
           <t>06-January-2025</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>1</v>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="3" t="n">
-        <v>0</v>
+      <c r="E7" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
@@ -650,7 +650,11 @@
       <c r="G7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
@@ -1333,13 +1337,13 @@
         </is>
       </c>
       <c r="C33" s="4" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D33" s="4" t="n">
         <v>0</v>
       </c>
       <c r="E33" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
current final working code ffor releasev1
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -732,30 +732,34 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="n">
+      <c r="A15" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="inlineStr">
+      <c r="B15" s="3" t="inlineStr">
         <is>
           <t>2025-01-06</t>
         </is>
       </c>
       <c r="C15" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="n">
@@ -1103,11 +1107,11 @@
         <v>0</v>
       </c>
       <c r="G28" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Annual Leave</t>
         </is>
       </c>
     </row>
@@ -1446,19 +1450,19 @@
         </is>
       </c>
       <c r="C41" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>3</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1509,7 +1513,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>04 - February - 2025</t>
+          <t>06 - February - 2025</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">

</xml_diff>

<commit_message>
Dont overwrite PH or weekends in timesheet
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -620,30 +620,34 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>2025-01-02</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>Annual Leave</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="n">
@@ -762,108 +766,124 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="n">
+      <c r="A16" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B16" s="4" t="inlineStr">
+      <c r="B16" s="3" t="inlineStr">
         <is>
           <t>2025-01-07</t>
         </is>
       </c>
       <c r="C16" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="n">
+      <c r="A17" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B17" s="4" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>2025-01-08</t>
         </is>
       </c>
       <c r="C17" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B18" s="4" t="inlineStr">
+      <c r="B18" s="3" t="inlineStr">
         <is>
           <t>2025-01-09</t>
         </is>
       </c>
       <c r="C18" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="n">
+      <c r="A19" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="4" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr">
         <is>
           <t>2025-01-10</t>
         </is>
       </c>
       <c r="C19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
@@ -1107,11 +1127,11 @@
         <v>0</v>
       </c>
       <c r="G28" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>Annual Leave</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -1450,13 +1470,13 @@
         </is>
       </c>
       <c r="C41" s="5" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>3</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F41" s="5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Added style changes working fine
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -469,35 +469,35 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PO Ref</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>GVT000ECI24000829</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Contractor</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>PALO IT</t>
+        </is>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PO Ref</t>
+          <t>PO Date</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>GVT000ECI24000829</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Contractor</t>
-        </is>
-      </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>PALO IT</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>PO Date</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>1 May 24 - 30 Apr 25</t>
         </is>
@@ -536,16 +536,20 @@
           <t>DevOps Engineer - II</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Group/Specialization</t>
         </is>
       </c>
-      <c r="E7" s="1" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>Consultant</t>
         </is>
       </c>
+      <c r="E8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -620,34 +624,30 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>2025-01-02</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3" t="inlineStr">
-        <is>
-          <t>Annual Leave</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="n">
@@ -946,30 +946,34 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="n">
+      <c r="A22" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B22" s="4" t="inlineStr">
+      <c r="B22" s="3" t="inlineStr">
         <is>
           <t>2025-01-13</t>
         </is>
       </c>
       <c r="C22" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n">
@@ -1476,13 +1480,13 @@
         <v>3</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G41" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">

</xml_diff>

<commit_message>
Added the format for rows correctly
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,167 +551,137 @@
       </c>
       <c r="E8" s="1" t="n"/>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>At Work</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>Public Holiday</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>Sick Leave</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t>Childcare Leave</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr">
+      <c r="G10" s="2" t="inlineStr">
         <is>
           <t>Annual Leave</t>
         </is>
       </c>
-      <c r="H9" s="2" t="inlineStr">
+      <c r="H10" s="2" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>2025-01-01</t>
         </is>
       </c>
-      <c r="C10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3" t="inlineStr">
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
         <is>
           <t>New Year's Day</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>2025-01-02</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>2025-01-02</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B13" s="4" t="inlineStr">
         <is>
           <t>2025-01-03</t>
         </is>
       </c>
-      <c r="C12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>2025-01-04</t>
-        </is>
-      </c>
       <c r="C13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>2025-01-05</t>
+          <t>2025-01-04</t>
         </is>
       </c>
       <c r="C14" s="3" t="n">
@@ -731,197 +701,177 @@
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>2025-01-05</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B16" s="4" t="inlineStr">
         <is>
           <t>2025-01-06</t>
         </is>
       </c>
-      <c r="C15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3" t="inlineStr">
-        <is>
-          <t>Sick Leave</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="n">
+      <c r="C16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B17" s="4" t="inlineStr">
         <is>
           <t>2025-01-07</t>
         </is>
       </c>
-      <c r="C16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3" t="inlineStr">
-        <is>
-          <t>Sick Leave</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="n">
+      <c r="C17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B18" s="4" t="inlineStr">
         <is>
           <t>2025-01-08</t>
         </is>
       </c>
-      <c r="C17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3" t="inlineStr">
-        <is>
-          <t>Sick Leave</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="n">
+      <c r="C18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B19" s="4" t="inlineStr">
         <is>
           <t>2025-01-09</t>
         </is>
       </c>
-      <c r="C18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3" t="inlineStr">
-        <is>
-          <t>Sick Leave</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="n">
+      <c r="C19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="3" t="inlineStr">
+      <c r="B20" s="4" t="inlineStr">
         <is>
           <t>2025-01-10</t>
         </is>
       </c>
-      <c r="C19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3" t="inlineStr">
-        <is>
-          <t>Sick Leave</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="B20" s="3" t="inlineStr">
-        <is>
-          <t>2025-01-11</t>
-        </is>
-      </c>
       <c r="C20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>2025-01-12</t>
+          <t>2025-01-11</t>
         </is>
       </c>
       <c r="C21" s="3" t="n">
@@ -941,17 +891,17 @@
       </c>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-12</t>
         </is>
       </c>
       <c r="C22" s="3" t="n">
@@ -961,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="3" t="n">
         <v>0</v>
@@ -971,17 +921,17 @@
       </c>
       <c r="H22" s="3" t="inlineStr">
         <is>
-          <t>Sick Leave</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-13</t>
         </is>
       </c>
       <c r="C23" s="3" t="n">
@@ -1003,11 +953,11 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>2025-01-15</t>
+          <t>2025-01-14</t>
         </is>
       </c>
       <c r="C24" s="3" t="n">
@@ -1029,11 +979,11 @@
     </row>
     <row r="25">
       <c r="A25" s="4" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>2025-01-16</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="C25" s="3" t="n">
@@ -1055,123 +1005,123 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>2025-01-16</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B26" s="4" t="inlineStr">
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>2025-01-17</t>
         </is>
       </c>
-      <c r="C26" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="4" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="3" t="n">
-        <v>18</v>
-      </c>
-      <c r="B27" s="3" t="inlineStr">
-        <is>
-          <t>2025-01-18</t>
-        </is>
-      </c>
       <c r="C27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>2025-01-18</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="B28" s="3" t="inlineStr">
+      <c r="B29" s="3" t="inlineStr">
         <is>
           <t>2025-01-19</t>
         </is>
       </c>
-      <c r="C28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="3" t="inlineStr">
+      <c r="C29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B29" s="4" t="inlineStr">
-        <is>
-          <t>2025-01-20</t>
-        </is>
-      </c>
-      <c r="C29" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="4" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>2025-01-21</t>
+          <t>2025-01-20</t>
         </is>
       </c>
       <c r="C30" s="3" t="n">
@@ -1193,11 +1143,11 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>2025-01-22</t>
+          <t>2025-01-21</t>
         </is>
       </c>
       <c r="C31" s="3" t="n">
@@ -1219,11 +1169,11 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>2025-01-23</t>
+          <t>2025-01-22</t>
         </is>
       </c>
       <c r="C32" s="3" t="n">
@@ -1245,307 +1195,339 @@
     </row>
     <row r="33">
       <c r="A33" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>2025-01-23</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B33" s="4" t="inlineStr">
+      <c r="B34" s="4" t="inlineStr">
         <is>
           <t>2025-01-24</t>
         </is>
       </c>
-      <c r="C33" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="4" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="n">
-        <v>25</v>
-      </c>
-      <c r="B34" s="3" t="inlineStr">
-        <is>
-          <t>2025-01-25</t>
-        </is>
-      </c>
       <c r="C34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>2025-01-25</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="B35" s="3" t="inlineStr">
+      <c r="B36" s="3" t="inlineStr">
         <is>
           <t>2025-01-26</t>
         </is>
       </c>
-      <c r="C35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3" t="inlineStr">
+      <c r="C36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="4" t="n">
-        <v>27</v>
-      </c>
-      <c r="B36" s="4" t="inlineStr">
-        <is>
-          <t>2025-01-27</t>
-        </is>
-      </c>
-      <c r="C36" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="4" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>2025-01-27</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="B37" s="4" t="inlineStr">
+      <c r="B38" s="4" t="inlineStr">
         <is>
           <t>2025-01-28</t>
         </is>
       </c>
-      <c r="C37" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="4" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="n">
-        <v>29</v>
-      </c>
-      <c r="B38" s="3" t="inlineStr">
-        <is>
-          <t>2025-01-29</t>
-        </is>
-      </c>
       <c r="C38" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="3" t="inlineStr">
-        <is>
-          <t>Chinese New Year (1st Day)</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>2025-01-29</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>Chinese New Year (1st Day)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="B39" s="3" t="inlineStr">
+      <c r="B40" s="3" t="inlineStr">
         <is>
           <t>2025-01-30</t>
         </is>
       </c>
-      <c r="C39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="3" t="inlineStr">
+      <c r="C40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
         <is>
           <t>Chinese New Year (2nd Day)</t>
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="4" t="n">
+    <row r="41">
+      <c r="A41" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="B40" s="4" t="inlineStr">
+      <c r="B41" s="4" t="inlineStr">
         <is>
           <t>2025-01-31</t>
         </is>
       </c>
-      <c r="C40" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D40" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="4" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="5" t="inlineStr">
+      <c r="C41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="5" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C41" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="D41" s="5" t="n">
+      <c r="C44" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="D44" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E41" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F41" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="E44" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
         <is>
           <t>Officer</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Signature</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Shamik Guha Ray</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>06 - February - 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
         <is>
           <t>Reporting Officer</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>Deepu Joseph</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="53">
+      <c r="A53" t="inlineStr">
         <is>
           <t>Signature</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Shamik Guha Ray</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Signature</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="B53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>06 - February - 2025</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed style for header --final
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,9 +27,13 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00000000"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -42,14 +46,47 @@
         <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E2EFDA"/>
+        <bgColor rgb="00E2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9E1F2"/>
+        <bgColor rgb="00D9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <bottom style="medium"/>
     </border>
     <border>
       <left style="thin"/>
@@ -61,19 +98,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -485,7 +534,7 @@
           <t>Contractor</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>PALO IT</t>
         </is>
@@ -562,17 +611,17 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>At Work</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="D10" s="4" t="inlineStr">
         <is>
           <t>Public Holiday</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="E10" s="5" t="inlineStr">
         <is>
           <t>Sick Leave</t>
         </is>
@@ -582,7 +631,7 @@
           <t>Childcare Leave</t>
         </is>
       </c>
-      <c r="G10" s="2" t="inlineStr">
+      <c r="G10" s="6" t="inlineStr">
         <is>
           <t>Annual Leave</t>
         </is>
@@ -594,874 +643,874 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="A11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>2025-01-01</t>
         </is>
       </c>
-      <c r="C11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3" t="inlineStr">
+      <c r="C11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7" t="inlineStr">
         <is>
           <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="n">
+      <c r="A12" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B12" s="8" t="inlineStr">
         <is>
           <t>2025-01-02</t>
         </is>
       </c>
-      <c r="C12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4" t="inlineStr"/>
+      <c r="C12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="n">
+      <c r="A13" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="4" t="inlineStr">
+      <c r="B13" s="8" t="inlineStr">
         <is>
           <t>2025-01-03</t>
         </is>
       </c>
-      <c r="C13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4" t="inlineStr"/>
+      <c r="C13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" s="7" t="inlineStr">
         <is>
           <t>2025-01-04</t>
         </is>
       </c>
-      <c r="C14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3" t="inlineStr">
+      <c r="C14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" s="7" t="inlineStr">
         <is>
           <t>2025-01-05</t>
         </is>
       </c>
-      <c r="C15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3" t="inlineStr">
+      <c r="C15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="n">
+      <c r="A16" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="4" t="inlineStr">
+      <c r="B16" s="8" t="inlineStr">
         <is>
           <t>2025-01-06</t>
         </is>
       </c>
-      <c r="C16" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4" t="inlineStr"/>
+      <c r="C16" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="n">
+      <c r="A17" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="4" t="inlineStr">
+      <c r="B17" s="8" t="inlineStr">
         <is>
           <t>2025-01-07</t>
         </is>
       </c>
-      <c r="C17" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4" t="inlineStr"/>
+      <c r="C17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="4" t="inlineStr">
+      <c r="B18" s="8" t="inlineStr">
         <is>
           <t>2025-01-08</t>
         </is>
       </c>
-      <c r="C18" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4" t="inlineStr"/>
+      <c r="C18" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="8" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="n">
+      <c r="A19" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="4" t="inlineStr">
+      <c r="B19" s="8" t="inlineStr">
         <is>
           <t>2025-01-09</t>
         </is>
       </c>
-      <c r="C19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4" t="inlineStr"/>
+      <c r="C19" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="n">
+      <c r="A20" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="4" t="inlineStr">
+      <c r="B20" s="8" t="inlineStr">
         <is>
           <t>2025-01-10</t>
         </is>
       </c>
-      <c r="C20" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="4" t="inlineStr"/>
+      <c r="C20" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" s="7" t="inlineStr">
         <is>
           <t>2025-01-11</t>
         </is>
       </c>
-      <c r="C21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3" t="inlineStr">
+      <c r="C21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B22" s="7" t="inlineStr">
         <is>
           <t>2025-01-12</t>
         </is>
       </c>
-      <c r="C22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3" t="inlineStr">
+      <c r="C22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="n">
+      <c r="A23" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="4" t="inlineStr">
+      <c r="B23" s="8" t="inlineStr">
         <is>
           <t>2025-01-13</t>
         </is>
       </c>
-      <c r="C23" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="4" t="inlineStr"/>
+      <c r="C23" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="8" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="n">
+      <c r="A24" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="4" t="inlineStr">
+      <c r="B24" s="8" t="inlineStr">
         <is>
           <t>2025-01-14</t>
         </is>
       </c>
-      <c r="C24" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="4" t="inlineStr"/>
+      <c r="C24" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="8" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n">
+      <c r="A25" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="B25" s="8" t="inlineStr">
         <is>
           <t>2025-01-15</t>
         </is>
       </c>
-      <c r="C25" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="4" t="inlineStr"/>
+      <c r="C25" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n">
+      <c r="A26" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="4" t="inlineStr">
+      <c r="B26" s="8" t="inlineStr">
         <is>
           <t>2025-01-16</t>
         </is>
       </c>
-      <c r="C26" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="4" t="inlineStr"/>
+      <c r="C26" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="8" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n">
+      <c r="A27" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="4" t="inlineStr">
+      <c r="B27" s="8" t="inlineStr">
         <is>
           <t>2025-01-17</t>
         </is>
       </c>
-      <c r="C27" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="4" t="inlineStr"/>
+      <c r="C27" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="B28" s="3" t="inlineStr">
+      <c r="B28" s="7" t="inlineStr">
         <is>
           <t>2025-01-18</t>
         </is>
       </c>
-      <c r="C28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="3" t="inlineStr">
+      <c r="C28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="7" t="n">
         <v>19</v>
       </c>
-      <c r="B29" s="3" t="inlineStr">
+      <c r="B29" s="7" t="inlineStr">
         <is>
           <t>2025-01-19</t>
         </is>
       </c>
-      <c r="C29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3" t="inlineStr">
+      <c r="C29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="7" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n">
+      <c r="A30" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="B30" s="4" t="inlineStr">
+      <c r="B30" s="8" t="inlineStr">
         <is>
           <t>2025-01-20</t>
         </is>
       </c>
-      <c r="C30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="4" t="inlineStr"/>
+      <c r="C30" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="8" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n">
+      <c r="A31" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="B31" s="4" t="inlineStr">
+      <c r="B31" s="8" t="inlineStr">
         <is>
           <t>2025-01-21</t>
         </is>
       </c>
-      <c r="C31" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="4" t="inlineStr"/>
+      <c r="C31" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="8" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="n">
+      <c r="A32" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="B32" s="4" t="inlineStr">
+      <c r="B32" s="8" t="inlineStr">
         <is>
           <t>2025-01-22</t>
         </is>
       </c>
-      <c r="C32" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="4" t="inlineStr"/>
+      <c r="C32" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="8" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="n">
+      <c r="A33" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="B33" s="4" t="inlineStr">
+      <c r="B33" s="8" t="inlineStr">
         <is>
           <t>2025-01-23</t>
         </is>
       </c>
-      <c r="C33" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="4" t="inlineStr"/>
+      <c r="C33" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="8" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="n">
+      <c r="A34" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="B34" s="4" t="inlineStr">
+      <c r="B34" s="8" t="inlineStr">
         <is>
           <t>2025-01-24</t>
         </is>
       </c>
-      <c r="C34" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="4" t="inlineStr"/>
+      <c r="C34" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="8" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="n">
+      <c r="A35" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="B35" s="3" t="inlineStr">
+      <c r="B35" s="7" t="inlineStr">
         <is>
           <t>2025-01-25</t>
         </is>
       </c>
-      <c r="C35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3" t="inlineStr">
+      <c r="C35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="n">
+      <c r="A36" s="7" t="n">
         <v>26</v>
       </c>
-      <c r="B36" s="3" t="inlineStr">
+      <c r="B36" s="7" t="inlineStr">
         <is>
           <t>2025-01-26</t>
         </is>
       </c>
-      <c r="C36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="3" t="inlineStr">
+      <c r="C36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="n">
+      <c r="A37" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="B37" s="4" t="inlineStr">
+      <c r="B37" s="8" t="inlineStr">
         <is>
           <t>2025-01-27</t>
         </is>
       </c>
-      <c r="C37" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="4" t="inlineStr"/>
+      <c r="C37" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="8" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="n">
+      <c r="A38" s="8" t="n">
         <v>28</v>
       </c>
-      <c r="B38" s="4" t="inlineStr">
+      <c r="B38" s="8" t="inlineStr">
         <is>
           <t>2025-01-28</t>
         </is>
       </c>
-      <c r="C38" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="4" t="inlineStr"/>
+      <c r="C38" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="8" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="n">
+      <c r="A39" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="B39" s="3" t="inlineStr">
+      <c r="B39" s="7" t="inlineStr">
         <is>
           <t>2025-01-29</t>
         </is>
       </c>
-      <c r="C39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="3" t="inlineStr">
+      <c r="C39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="7" t="inlineStr">
         <is>
           <t>Chinese New Year (1st Day)</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="n">
+      <c r="A40" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="B40" s="3" t="inlineStr">
+      <c r="B40" s="7" t="inlineStr">
         <is>
           <t>2025-01-30</t>
         </is>
       </c>
-      <c r="C40" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="3" t="inlineStr">
+      <c r="C40" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="7" t="inlineStr">
         <is>
           <t>Chinese New Year (2nd Day)</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="n">
+      <c r="A41" s="8" t="n">
         <v>31</v>
       </c>
-      <c r="B41" s="4" t="inlineStr">
+      <c r="B41" s="8" t="inlineStr">
         <is>
           <t>2025-01-31</t>
         </is>
       </c>
-      <c r="C41" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="4" t="inlineStr"/>
+      <c r="C41" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="8" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" s="5" t="inlineStr">
+      <c r="A44" s="9" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C44" s="5" t="n">
+      <c r="C44" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="D44" s="5" t="n">
+      <c r="D44" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="E44" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="5" t="n">
+      <c r="E44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="9" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add correct format of style before fxing final style
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -119,13 +119,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -657,34 +657,22 @@
           <t>01-January-2025</t>
         </is>
       </c>
-      <c r="C11" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D11" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G11" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H11" s="9" t="inlineStr">
-        <is>
-          <t>New Year's Day</t>
+      <c r="C11" s="8" t="inlineStr"/>
+      <c r="D11" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F11" s="8" t="inlineStr"/>
+      <c r="G11" s="8" t="inlineStr"/>
+      <c r="H11" s="10" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
         </is>
       </c>
     </row>
@@ -697,34 +685,22 @@
           <t>02-January-2025</t>
         </is>
       </c>
-      <c r="C12" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D12" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F12" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G12" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H12" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C12" s="8" t="inlineStr"/>
+      <c r="D12" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F12" s="8" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr"/>
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
         </is>
       </c>
     </row>
@@ -737,34 +713,22 @@
           <t>03-January-2025</t>
         </is>
       </c>
-      <c r="C13" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G13" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H13" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C13" s="8" t="inlineStr"/>
+      <c r="D13" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E13" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr"/>
+      <c r="G13" s="8" t="inlineStr"/>
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
         </is>
       </c>
     </row>
@@ -777,34 +741,22 @@
           <t>04-January-2025</t>
         </is>
       </c>
-      <c r="C14" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D14" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E14" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F14" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G14" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H14" s="9" t="inlineStr">
-        <is>
-          <t>Saturday</t>
+      <c r="C14" s="8" t="inlineStr"/>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F14" s="8" t="inlineStr"/>
+      <c r="G14" s="8" t="inlineStr"/>
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
         </is>
       </c>
     </row>
@@ -817,34 +769,22 @@
           <t>05-January-2025</t>
         </is>
       </c>
-      <c r="C15" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D15" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E15" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F15" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G15" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H15" s="9" t="inlineStr">
-        <is>
-          <t>Sunday</t>
+      <c r="C15" s="8" t="inlineStr"/>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F15" s="8" t="inlineStr"/>
+      <c r="G15" s="8" t="inlineStr"/>
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
         </is>
       </c>
     </row>
@@ -857,34 +797,22 @@
           <t>06-January-2025</t>
         </is>
       </c>
-      <c r="C16" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D16" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E16" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F16" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G16" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H16" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C16" s="8" t="inlineStr"/>
+      <c r="D16" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr"/>
+      <c r="G16" s="8" t="inlineStr"/>
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
         </is>
       </c>
     </row>
@@ -897,34 +825,22 @@
           <t>07-January-2025</t>
         </is>
       </c>
-      <c r="C17" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D17" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F17" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G17" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H17" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C17" s="8" t="inlineStr"/>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E17" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr"/>
+      <c r="G17" s="8" t="inlineStr"/>
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>Sick Leave</t>
         </is>
       </c>
     </row>
@@ -937,31 +853,19 @@
           <t>08-January-2025</t>
         </is>
       </c>
-      <c r="C18" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D18" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E18" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F18" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G18" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C18" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D18" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" s="8" t="inlineStr"/>
+      <c r="F18" s="8" t="inlineStr"/>
+      <c r="G18" s="8" t="inlineStr"/>
       <c r="H18" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -977,31 +881,19 @@
           <t>09-January-2025</t>
         </is>
       </c>
-      <c r="C19" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D19" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E19" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F19" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G19" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C19" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D19" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" s="8" t="inlineStr"/>
+      <c r="F19" s="8" t="inlineStr"/>
+      <c r="G19" s="8" t="inlineStr"/>
       <c r="H19" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1017,31 +909,19 @@
           <t>10-January-2025</t>
         </is>
       </c>
-      <c r="C20" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D20" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E20" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F20" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G20" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C20" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" s="8" t="inlineStr"/>
+      <c r="F20" s="8" t="inlineStr"/>
+      <c r="G20" s="8" t="inlineStr"/>
       <c r="H20" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1057,32 +937,16 @@
           <t>11-January-2025</t>
         </is>
       </c>
-      <c r="C21" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D21" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E21" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F21" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G21" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H21" s="9" t="inlineStr">
+      <c r="C21" s="8" t="inlineStr"/>
+      <c r="D21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="8" t="inlineStr"/>
+      <c r="F21" s="8" t="inlineStr"/>
+      <c r="G21" s="8" t="inlineStr"/>
+      <c r="H21" s="10" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
@@ -1097,32 +961,16 @@
           <t>12-January-2025</t>
         </is>
       </c>
-      <c r="C22" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D22" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E22" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F22" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G22" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H22" s="9" t="inlineStr">
+      <c r="C22" s="8" t="inlineStr"/>
+      <c r="D22" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" s="8" t="inlineStr"/>
+      <c r="F22" s="8" t="inlineStr"/>
+      <c r="G22" s="8" t="inlineStr"/>
+      <c r="H22" s="10" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
@@ -1137,31 +985,19 @@
           <t>13-January-2025</t>
         </is>
       </c>
-      <c r="C23" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D23" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E23" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F23" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G23" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C23" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="inlineStr"/>
+      <c r="F23" s="8" t="inlineStr"/>
+      <c r="G23" s="8" t="inlineStr"/>
       <c r="H23" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1177,31 +1013,19 @@
           <t>14-January-2025</t>
         </is>
       </c>
-      <c r="C24" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D24" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F24" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G24" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C24" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D24" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr"/>
+      <c r="F24" s="8" t="inlineStr"/>
+      <c r="G24" s="8" t="inlineStr"/>
       <c r="H24" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1217,31 +1041,19 @@
           <t>15-January-2025</t>
         </is>
       </c>
-      <c r="C25" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D25" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E25" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F25" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G25" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C25" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" s="8" t="inlineStr"/>
+      <c r="F25" s="8" t="inlineStr"/>
+      <c r="G25" s="8" t="inlineStr"/>
       <c r="H25" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1257,31 +1069,19 @@
           <t>16-January-2025</t>
         </is>
       </c>
-      <c r="C26" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D26" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E26" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F26" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G26" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C26" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D26" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="8" t="inlineStr"/>
+      <c r="F26" s="8" t="inlineStr"/>
+      <c r="G26" s="8" t="inlineStr"/>
       <c r="H26" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1297,31 +1097,19 @@
           <t>17-January-2025</t>
         </is>
       </c>
-      <c r="C27" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D27" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E27" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F27" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G27" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C27" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" s="8" t="inlineStr"/>
+      <c r="F27" s="8" t="inlineStr"/>
+      <c r="G27" s="8" t="inlineStr"/>
       <c r="H27" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1337,32 +1125,16 @@
           <t>18-January-2025</t>
         </is>
       </c>
-      <c r="C28" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D28" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E28" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F28" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G28" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H28" s="9" t="inlineStr">
+      <c r="C28" s="8" t="inlineStr"/>
+      <c r="D28" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="8" t="inlineStr"/>
+      <c r="F28" s="8" t="inlineStr"/>
+      <c r="G28" s="8" t="inlineStr"/>
+      <c r="H28" s="10" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
@@ -1377,32 +1149,16 @@
           <t>19-January-2025</t>
         </is>
       </c>
-      <c r="C29" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D29" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E29" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F29" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G29" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H29" s="9" t="inlineStr">
+      <c r="C29" s="8" t="inlineStr"/>
+      <c r="D29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="8" t="inlineStr"/>
+      <c r="F29" s="8" t="inlineStr"/>
+      <c r="G29" s="8" t="inlineStr"/>
+      <c r="H29" s="10" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
@@ -1417,31 +1173,19 @@
           <t>20-January-2025</t>
         </is>
       </c>
-      <c r="C30" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D30" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E30" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F30" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G30" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C30" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D30" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" s="8" t="inlineStr"/>
+      <c r="F30" s="8" t="inlineStr"/>
+      <c r="G30" s="8" t="inlineStr"/>
       <c r="H30" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1457,31 +1201,19 @@
           <t>21-January-2025</t>
         </is>
       </c>
-      <c r="C31" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D31" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E31" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F31" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G31" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C31" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D31" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" s="8" t="inlineStr"/>
+      <c r="F31" s="8" t="inlineStr"/>
+      <c r="G31" s="8" t="inlineStr"/>
       <c r="H31" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1497,31 +1229,19 @@
           <t>22-January-2025</t>
         </is>
       </c>
-      <c r="C32" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D32" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E32" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F32" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G32" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C32" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D32" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="8" t="inlineStr"/>
+      <c r="F32" s="8" t="inlineStr"/>
+      <c r="G32" s="8" t="inlineStr"/>
       <c r="H32" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1537,31 +1257,19 @@
           <t>23-January-2025</t>
         </is>
       </c>
-      <c r="C33" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D33" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E33" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F33" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G33" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C33" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D33" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" s="8" t="inlineStr"/>
+      <c r="F33" s="8" t="inlineStr"/>
+      <c r="G33" s="8" t="inlineStr"/>
       <c r="H33" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1577,31 +1285,19 @@
           <t>24-January-2025</t>
         </is>
       </c>
-      <c r="C34" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D34" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E34" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F34" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G34" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C34" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D34" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr"/>
+      <c r="F34" s="8" t="inlineStr"/>
+      <c r="G34" s="8" t="inlineStr"/>
       <c r="H34" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1617,32 +1313,16 @@
           <t>25-January-2025</t>
         </is>
       </c>
-      <c r="C35" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D35" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E35" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F35" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G35" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H35" s="9" t="inlineStr">
+      <c r="C35" s="8" t="inlineStr"/>
+      <c r="D35" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="8" t="inlineStr"/>
+      <c r="F35" s="8" t="inlineStr"/>
+      <c r="G35" s="8" t="inlineStr"/>
+      <c r="H35" s="10" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
@@ -1657,32 +1337,16 @@
           <t>26-January-2025</t>
         </is>
       </c>
-      <c r="C36" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D36" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E36" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F36" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G36" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H36" s="9" t="inlineStr">
+      <c r="C36" s="8" t="inlineStr"/>
+      <c r="D36" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" s="8" t="inlineStr"/>
+      <c r="F36" s="8" t="inlineStr"/>
+      <c r="G36" s="8" t="inlineStr"/>
+      <c r="H36" s="10" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
@@ -1697,31 +1361,19 @@
           <t>27-January-2025</t>
         </is>
       </c>
-      <c r="C37" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D37" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E37" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F37" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G37" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C37" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D37" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" s="8" t="inlineStr"/>
+      <c r="F37" s="8" t="inlineStr"/>
+      <c r="G37" s="8" t="inlineStr"/>
       <c r="H37" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1737,31 +1389,19 @@
           <t>28-January-2025</t>
         </is>
       </c>
-      <c r="C38" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D38" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E38" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F38" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G38" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C38" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D38" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" s="8" t="inlineStr"/>
+      <c r="F38" s="8" t="inlineStr"/>
+      <c r="G38" s="8" t="inlineStr"/>
       <c r="H38" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1777,32 +1417,16 @@
           <t>29-January-2025</t>
         </is>
       </c>
-      <c r="C39" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D39" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="E39" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F39" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G39" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H39" s="9" t="inlineStr">
+      <c r="C39" s="8" t="inlineStr"/>
+      <c r="D39" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E39" s="8" t="inlineStr"/>
+      <c r="F39" s="8" t="inlineStr"/>
+      <c r="G39" s="8" t="inlineStr"/>
+      <c r="H39" s="10" t="inlineStr">
         <is>
           <t>Chinese New Year (1st Day)</t>
         </is>
@@ -1817,32 +1441,16 @@
           <t>30-January-2025</t>
         </is>
       </c>
-      <c r="C40" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D40" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="E40" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F40" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G40" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H40" s="9" t="inlineStr">
+      <c r="C40" s="8" t="inlineStr"/>
+      <c r="D40" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E40" s="8" t="inlineStr"/>
+      <c r="F40" s="8" t="inlineStr"/>
+      <c r="G40" s="8" t="inlineStr"/>
+      <c r="H40" s="10" t="inlineStr">
         <is>
           <t>Chinese New Year (2nd Day)</t>
         </is>
@@ -1857,31 +1465,19 @@
           <t>31-January-2025</t>
         </is>
       </c>
-      <c r="C41" s="8" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D41" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E41" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F41" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G41" s="8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="C41" s="9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D41" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" s="8" t="inlineStr"/>
+      <c r="F41" s="8" t="inlineStr"/>
+      <c r="G41" s="8" t="inlineStr"/>
       <c r="H41" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1896,7 +1492,7 @@
       </c>
       <c r="C44" s="11" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>16.0</t>
         </is>
       </c>
       <c r="D44" s="11" t="inlineStr">
@@ -1906,7 +1502,7 @@
       </c>
       <c r="E44" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="F44" s="11" t="inlineStr">

</xml_diff>

<commit_message>
all styles Finally done
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,10 +30,13 @@
       <color rgb="00000000"/>
     </font>
     <font>
+      <color rgb="00FF0000"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -76,6 +79,12 @@
         <bgColor rgb="00D9E1F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -98,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -126,16 +135,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -704,7 +719,7 @@
       <c r="E12" s="10" t="inlineStr"/>
       <c r="F12" s="10" t="inlineStr"/>
       <c r="G12" s="10" t="inlineStr"/>
-      <c r="H12" s="3" t="inlineStr">
+      <c r="H12" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -732,7 +747,7 @@
       <c r="E13" s="10" t="inlineStr"/>
       <c r="F13" s="10" t="inlineStr"/>
       <c r="G13" s="10" t="inlineStr"/>
-      <c r="H13" s="3" t="inlineStr">
+      <c r="H13" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -808,7 +823,7 @@
       <c r="E16" s="10" t="inlineStr"/>
       <c r="F16" s="10" t="inlineStr"/>
       <c r="G16" s="10" t="inlineStr"/>
-      <c r="H16" s="3" t="inlineStr">
+      <c r="H16" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -836,7 +851,7 @@
       <c r="E17" s="10" t="inlineStr"/>
       <c r="F17" s="10" t="inlineStr"/>
       <c r="G17" s="10" t="inlineStr"/>
-      <c r="H17" s="3" t="inlineStr">
+      <c r="H17" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -864,7 +879,7 @@
       <c r="E18" s="10" t="inlineStr"/>
       <c r="F18" s="10" t="inlineStr"/>
       <c r="G18" s="10" t="inlineStr"/>
-      <c r="H18" s="3" t="inlineStr">
+      <c r="H18" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -892,7 +907,7 @@
       <c r="E19" s="10" t="inlineStr"/>
       <c r="F19" s="10" t="inlineStr"/>
       <c r="G19" s="10" t="inlineStr"/>
-      <c r="H19" s="3" t="inlineStr">
+      <c r="H19" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -920,7 +935,7 @@
       <c r="E20" s="10" t="inlineStr"/>
       <c r="F20" s="10" t="inlineStr"/>
       <c r="G20" s="10" t="inlineStr"/>
-      <c r="H20" s="3" t="inlineStr">
+      <c r="H20" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -996,7 +1011,7 @@
       <c r="E23" s="10" t="inlineStr"/>
       <c r="F23" s="10" t="inlineStr"/>
       <c r="G23" s="10" t="inlineStr"/>
-      <c r="H23" s="3" t="inlineStr">
+      <c r="H23" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1024,7 +1039,7 @@
       <c r="E24" s="10" t="inlineStr"/>
       <c r="F24" s="10" t="inlineStr"/>
       <c r="G24" s="10" t="inlineStr"/>
-      <c r="H24" s="3" t="inlineStr">
+      <c r="H24" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1052,7 +1067,7 @@
       <c r="E25" s="10" t="inlineStr"/>
       <c r="F25" s="10" t="inlineStr"/>
       <c r="G25" s="10" t="inlineStr"/>
-      <c r="H25" s="3" t="inlineStr">
+      <c r="H25" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1080,7 +1095,7 @@
       <c r="E26" s="10" t="inlineStr"/>
       <c r="F26" s="10" t="inlineStr"/>
       <c r="G26" s="10" t="inlineStr"/>
-      <c r="H26" s="3" t="inlineStr">
+      <c r="H26" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1108,7 +1123,7 @@
       <c r="E27" s="10" t="inlineStr"/>
       <c r="F27" s="10" t="inlineStr"/>
       <c r="G27" s="10" t="inlineStr"/>
-      <c r="H27" s="3" t="inlineStr">
+      <c r="H27" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1184,7 +1199,7 @@
       <c r="E30" s="10" t="inlineStr"/>
       <c r="F30" s="10" t="inlineStr"/>
       <c r="G30" s="10" t="inlineStr"/>
-      <c r="H30" s="3" t="inlineStr">
+      <c r="H30" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1212,7 +1227,7 @@
       <c r="E31" s="10" t="inlineStr"/>
       <c r="F31" s="10" t="inlineStr"/>
       <c r="G31" s="10" t="inlineStr"/>
-      <c r="H31" s="3" t="inlineStr">
+      <c r="H31" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1240,7 +1255,7 @@
       <c r="E32" s="10" t="inlineStr"/>
       <c r="F32" s="10" t="inlineStr"/>
       <c r="G32" s="10" t="inlineStr"/>
-      <c r="H32" s="3" t="inlineStr">
+      <c r="H32" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1268,7 +1283,7 @@
       <c r="E33" s="10" t="inlineStr"/>
       <c r="F33" s="10" t="inlineStr"/>
       <c r="G33" s="10" t="inlineStr"/>
-      <c r="H33" s="3" t="inlineStr">
+      <c r="H33" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1296,7 +1311,7 @@
       <c r="E34" s="10" t="inlineStr"/>
       <c r="F34" s="10" t="inlineStr"/>
       <c r="G34" s="10" t="inlineStr"/>
-      <c r="H34" s="3" t="inlineStr">
+      <c r="H34" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1372,7 +1387,7 @@
       <c r="E37" s="10" t="inlineStr"/>
       <c r="F37" s="10" t="inlineStr"/>
       <c r="G37" s="10" t="inlineStr"/>
-      <c r="H37" s="3" t="inlineStr">
+      <c r="H37" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1400,7 +1415,7 @@
       <c r="E38" s="10" t="inlineStr"/>
       <c r="F38" s="10" t="inlineStr"/>
       <c r="G38" s="10" t="inlineStr"/>
-      <c r="H38" s="3" t="inlineStr">
+      <c r="H38" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1476,43 +1491,59 @@
       <c r="E41" s="10" t="inlineStr"/>
       <c r="F41" s="10" t="inlineStr"/>
       <c r="G41" s="10" t="inlineStr"/>
-      <c r="H41" s="3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H41" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="H42" s="14" t="n"/>
+    </row>
+    <row r="43">
+      <c r="H43" s="14" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="13" t="inlineStr">
+      <c r="A44" s="15" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C44" s="14" t="inlineStr">
+      <c r="C44" s="16" t="inlineStr">
         <is>
           <t>20.0</t>
         </is>
       </c>
-      <c r="D44" s="14" t="inlineStr">
+      <c r="D44" s="16" t="inlineStr">
         <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="E44" s="14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F44" s="14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G44" s="14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="E44" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F44" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" s="14" t="n"/>
+    </row>
+    <row r="45">
+      <c r="H45" s="14" t="n"/>
+    </row>
+    <row r="46">
+      <c r="H46" s="14" t="n"/>
+    </row>
+    <row r="47">
+      <c r="H47" s="14" t="n"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1520,11 +1551,12 @@
           <t>Officer</t>
         </is>
       </c>
-      <c r="B48" s="15" t="inlineStr">
+      <c r="B48" s="17" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
+      <c r="H48" s="14" t="n"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1532,11 +1564,12 @@
           <t>Signature</t>
         </is>
       </c>
-      <c r="B49" s="15" t="inlineStr">
+      <c r="B49" s="17" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
+      <c r="H49" s="14" t="n"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1544,11 +1577,15 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="B50" s="15" t="inlineStr">
+      <c r="B50" s="17" t="inlineStr">
         <is>
           <t>06 - February - 2025</t>
         </is>
       </c>
+      <c r="H50" s="14" t="n"/>
+    </row>
+    <row r="51">
+      <c r="H51" s="14" t="n"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1556,11 +1593,12 @@
           <t>Reporting Officer</t>
         </is>
       </c>
-      <c r="B52" s="15" t="inlineStr">
+      <c r="B52" s="17" t="inlineStr">
         <is>
           <t>Deepu Joseph</t>
         </is>
       </c>
+      <c r="H52" s="14" t="n"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">

</xml_diff>

<commit_message>
changes to style.py and fixed leave entries on ph n weekends
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -709,17 +709,17 @@
           <t>02-January-2025</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C12" s="10" t="inlineStr"/>
       <c r="D12" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E12" s="10" t="inlineStr"/>
+      <c r="E12" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F12" s="10" t="inlineStr"/>
       <c r="G12" s="10" t="inlineStr"/>
       <c r="H12" s="13" t="inlineStr">
@@ -737,17 +737,17 @@
           <t>03-January-2025</t>
         </is>
       </c>
-      <c r="C13" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C13" s="10" t="inlineStr"/>
       <c r="D13" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E13" s="10" t="inlineStr"/>
+      <c r="E13" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F13" s="10" t="inlineStr"/>
       <c r="G13" s="10" t="inlineStr"/>
       <c r="H13" s="13" t="inlineStr">
@@ -925,18 +925,18 @@
           <t>10-January-2025</t>
         </is>
       </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C20" s="10" t="inlineStr"/>
       <c r="D20" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E20" s="10" t="inlineStr"/>
-      <c r="F20" s="10" t="inlineStr"/>
+      <c r="F20" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="G20" s="10" t="inlineStr"/>
       <c r="H20" s="13" t="inlineStr">
         <is>
@@ -1001,18 +1001,18 @@
           <t>13-January-2025</t>
         </is>
       </c>
-      <c r="C23" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C23" s="10" t="inlineStr"/>
       <c r="D23" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E23" s="10" t="inlineStr"/>
-      <c r="F23" s="10" t="inlineStr"/>
+      <c r="F23" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="G23" s="10" t="inlineStr"/>
       <c r="H23" s="13" t="inlineStr">
         <is>
@@ -1029,18 +1029,18 @@
           <t>14-January-2025</t>
         </is>
       </c>
-      <c r="C24" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C24" s="10" t="inlineStr"/>
       <c r="D24" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E24" s="10" t="inlineStr"/>
-      <c r="F24" s="10" t="inlineStr"/>
+      <c r="F24" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="G24" s="10" t="inlineStr"/>
       <c r="H24" s="13" t="inlineStr">
         <is>
@@ -1057,18 +1057,18 @@
           <t>15-January-2025</t>
         </is>
       </c>
-      <c r="C25" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C25" s="10" t="inlineStr"/>
       <c r="D25" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E25" s="10" t="inlineStr"/>
-      <c r="F25" s="10" t="inlineStr"/>
+      <c r="F25" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="G25" s="10" t="inlineStr"/>
       <c r="H25" s="13" t="inlineStr">
         <is>
@@ -1085,19 +1085,23 @@
           <t>16-January-2025</t>
         </is>
       </c>
-      <c r="C26" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C26" s="10" t="inlineStr"/>
       <c r="D26" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E26" s="10" t="inlineStr"/>
-      <c r="F26" s="10" t="inlineStr"/>
-      <c r="G26" s="10" t="inlineStr"/>
+      <c r="F26" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="G26" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H26" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1113,19 +1117,23 @@
           <t>17-January-2025</t>
         </is>
       </c>
-      <c r="C27" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C27" s="10" t="inlineStr"/>
       <c r="D27" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E27" s="10" t="inlineStr"/>
-      <c r="F27" s="10" t="inlineStr"/>
-      <c r="G27" s="10" t="inlineStr"/>
+      <c r="F27" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="G27" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H27" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1189,11 +1197,7 @@
           <t>20-January-2025</t>
         </is>
       </c>
-      <c r="C30" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C30" s="10" t="inlineStr"/>
       <c r="D30" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1201,7 +1205,11 @@
       </c>
       <c r="E30" s="10" t="inlineStr"/>
       <c r="F30" s="10" t="inlineStr"/>
-      <c r="G30" s="10" t="inlineStr"/>
+      <c r="G30" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H30" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1217,11 +1225,7 @@
           <t>21-January-2025</t>
         </is>
       </c>
-      <c r="C31" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C31" s="10" t="inlineStr"/>
       <c r="D31" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1229,7 +1233,11 @@
       </c>
       <c r="E31" s="10" t="inlineStr"/>
       <c r="F31" s="10" t="inlineStr"/>
-      <c r="G31" s="10" t="inlineStr"/>
+      <c r="G31" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H31" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1245,11 +1253,7 @@
           <t>22-January-2025</t>
         </is>
       </c>
-      <c r="C32" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C32" s="10" t="inlineStr"/>
       <c r="D32" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1257,7 +1261,11 @@
       </c>
       <c r="E32" s="10" t="inlineStr"/>
       <c r="F32" s="10" t="inlineStr"/>
-      <c r="G32" s="10" t="inlineStr"/>
+      <c r="G32" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H32" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1273,11 +1281,7 @@
           <t>23-January-2025</t>
         </is>
       </c>
-      <c r="C33" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C33" s="10" t="inlineStr"/>
       <c r="D33" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1285,7 +1289,11 @@
       </c>
       <c r="E33" s="10" t="inlineStr"/>
       <c r="F33" s="10" t="inlineStr"/>
-      <c r="G33" s="10" t="inlineStr"/>
+      <c r="G33" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H33" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1301,11 +1309,7 @@
           <t>24-January-2025</t>
         </is>
       </c>
-      <c r="C34" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C34" s="10" t="inlineStr"/>
       <c r="D34" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1313,7 +1317,11 @@
       </c>
       <c r="E34" s="10" t="inlineStr"/>
       <c r="F34" s="10" t="inlineStr"/>
-      <c r="G34" s="10" t="inlineStr"/>
+      <c r="G34" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H34" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1377,11 +1385,7 @@
           <t>27-January-2025</t>
         </is>
       </c>
-      <c r="C37" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C37" s="10" t="inlineStr"/>
       <c r="D37" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1389,7 +1393,11 @@
       </c>
       <c r="E37" s="10" t="inlineStr"/>
       <c r="F37" s="10" t="inlineStr"/>
-      <c r="G37" s="10" t="inlineStr"/>
+      <c r="G37" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H37" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1405,11 +1413,7 @@
           <t>28-January-2025</t>
         </is>
       </c>
-      <c r="C38" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C38" s="10" t="inlineStr"/>
       <c r="D38" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1417,7 +1421,11 @@
       </c>
       <c r="E38" s="10" t="inlineStr"/>
       <c r="F38" s="10" t="inlineStr"/>
-      <c r="G38" s="10" t="inlineStr"/>
+      <c r="G38" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H38" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1481,11 +1489,7 @@
           <t>31-January-2025</t>
         </is>
       </c>
-      <c r="C41" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C41" s="10" t="inlineStr"/>
       <c r="D41" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1493,7 +1497,11 @@
       </c>
       <c r="E41" s="10" t="inlineStr"/>
       <c r="F41" s="10" t="inlineStr"/>
-      <c r="G41" s="10" t="inlineStr"/>
+      <c r="G41" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H41" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1514,7 +1522,7 @@
       </c>
       <c r="C44" s="16" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="D44" s="16" t="inlineStr">
@@ -1524,17 +1532,17 @@
       </c>
       <c r="E44" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="F44" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="G44" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H44" s="14" t="n"/>
@@ -1582,7 +1590,7 @@
       </c>
       <c r="B50" s="17" t="inlineStr">
         <is>
-          <t>06 - February - 2025</t>
+          <t>07 - February - 2025</t>
         </is>
       </c>
       <c r="H50" s="14" t="n"/>

</xml_diff>

<commit_message>
add new user handle
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -813,17 +813,17 @@
           <t>06-January-2025</t>
         </is>
       </c>
-      <c r="C16" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C16" s="10" t="inlineStr"/>
       <c r="D16" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E16" s="10" t="inlineStr"/>
+      <c r="E16" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F16" s="10" t="inlineStr"/>
       <c r="G16" s="10" t="inlineStr"/>
       <c r="H16" s="13" t="inlineStr">
@@ -841,17 +841,17 @@
           <t>07-January-2025</t>
         </is>
       </c>
-      <c r="C17" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C17" s="10" t="inlineStr"/>
       <c r="D17" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E17" s="10" t="inlineStr"/>
+      <c r="E17" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F17" s="10" t="inlineStr"/>
       <c r="G17" s="10" t="inlineStr"/>
       <c r="H17" s="13" t="inlineStr">
@@ -869,17 +869,17 @@
           <t>08-January-2025</t>
         </is>
       </c>
-      <c r="C18" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C18" s="10" t="inlineStr"/>
       <c r="D18" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E18" s="10" t="inlineStr"/>
+      <c r="E18" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F18" s="10" t="inlineStr"/>
       <c r="G18" s="10" t="inlineStr"/>
       <c r="H18" s="13" t="inlineStr">
@@ -897,17 +897,17 @@
           <t>09-January-2025</t>
         </is>
       </c>
-      <c r="C19" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C19" s="10" t="inlineStr"/>
       <c r="D19" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E19" s="10" t="inlineStr"/>
+      <c r="E19" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F19" s="10" t="inlineStr"/>
       <c r="G19" s="10" t="inlineStr"/>
       <c r="H19" s="13" t="inlineStr">
@@ -931,12 +931,12 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E20" s="10" t="inlineStr"/>
-      <c r="F20" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="E20" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F20" s="10" t="inlineStr"/>
       <c r="G20" s="10" t="inlineStr"/>
       <c r="H20" s="13" t="inlineStr">
         <is>
@@ -1001,18 +1001,18 @@
           <t>13-January-2025</t>
         </is>
       </c>
-      <c r="C23" s="10" t="inlineStr"/>
+      <c r="C23" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D23" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E23" s="10" t="inlineStr"/>
-      <c r="F23" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="F23" s="10" t="inlineStr"/>
       <c r="G23" s="10" t="inlineStr"/>
       <c r="H23" s="13" t="inlineStr">
         <is>
@@ -1029,18 +1029,18 @@
           <t>14-January-2025</t>
         </is>
       </c>
-      <c r="C24" s="10" t="inlineStr"/>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D24" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E24" s="10" t="inlineStr"/>
-      <c r="F24" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="F24" s="10" t="inlineStr"/>
       <c r="G24" s="10" t="inlineStr"/>
       <c r="H24" s="13" t="inlineStr">
         <is>
@@ -1057,18 +1057,18 @@
           <t>15-January-2025</t>
         </is>
       </c>
-      <c r="C25" s="10" t="inlineStr"/>
+      <c r="C25" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D25" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E25" s="10" t="inlineStr"/>
-      <c r="F25" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="F25" s="10" t="inlineStr"/>
       <c r="G25" s="10" t="inlineStr"/>
       <c r="H25" s="13" t="inlineStr">
         <is>
@@ -1085,23 +1085,19 @@
           <t>16-January-2025</t>
         </is>
       </c>
-      <c r="C26" s="10" t="inlineStr"/>
+      <c r="C26" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D26" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E26" s="10" t="inlineStr"/>
-      <c r="F26" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="G26" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="F26" s="10" t="inlineStr"/>
+      <c r="G26" s="10" t="inlineStr"/>
       <c r="H26" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1117,23 +1113,19 @@
           <t>17-January-2025</t>
         </is>
       </c>
-      <c r="C27" s="10" t="inlineStr"/>
+      <c r="C27" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D27" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E27" s="10" t="inlineStr"/>
-      <c r="F27" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="G27" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="F27" s="10" t="inlineStr"/>
+      <c r="G27" s="10" t="inlineStr"/>
       <c r="H27" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1197,7 +1189,11 @@
           <t>20-January-2025</t>
         </is>
       </c>
-      <c r="C30" s="10" t="inlineStr"/>
+      <c r="C30" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D30" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1205,11 +1201,7 @@
       </c>
       <c r="E30" s="10" t="inlineStr"/>
       <c r="F30" s="10" t="inlineStr"/>
-      <c r="G30" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G30" s="10" t="inlineStr"/>
       <c r="H30" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1225,7 +1217,11 @@
           <t>21-January-2025</t>
         </is>
       </c>
-      <c r="C31" s="10" t="inlineStr"/>
+      <c r="C31" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D31" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1233,11 +1229,7 @@
       </c>
       <c r="E31" s="10" t="inlineStr"/>
       <c r="F31" s="10" t="inlineStr"/>
-      <c r="G31" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G31" s="10" t="inlineStr"/>
       <c r="H31" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1253,7 +1245,11 @@
           <t>22-January-2025</t>
         </is>
       </c>
-      <c r="C32" s="10" t="inlineStr"/>
+      <c r="C32" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D32" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1261,11 +1257,7 @@
       </c>
       <c r="E32" s="10" t="inlineStr"/>
       <c r="F32" s="10" t="inlineStr"/>
-      <c r="G32" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G32" s="10" t="inlineStr"/>
       <c r="H32" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1281,7 +1273,11 @@
           <t>23-January-2025</t>
         </is>
       </c>
-      <c r="C33" s="10" t="inlineStr"/>
+      <c r="C33" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D33" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1289,11 +1285,7 @@
       </c>
       <c r="E33" s="10" t="inlineStr"/>
       <c r="F33" s="10" t="inlineStr"/>
-      <c r="G33" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G33" s="10" t="inlineStr"/>
       <c r="H33" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1316,12 +1308,12 @@
         </is>
       </c>
       <c r="E34" s="10" t="inlineStr"/>
-      <c r="F34" s="10" t="inlineStr"/>
-      <c r="G34" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="F34" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="G34" s="10" t="inlineStr"/>
       <c r="H34" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1392,12 +1384,12 @@
         </is>
       </c>
       <c r="E37" s="10" t="inlineStr"/>
-      <c r="F37" s="10" t="inlineStr"/>
-      <c r="G37" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="F37" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="G37" s="10" t="inlineStr"/>
       <c r="H37" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1413,7 +1405,11 @@
           <t>28-January-2025</t>
         </is>
       </c>
-      <c r="C38" s="10" t="inlineStr"/>
+      <c r="C38" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D38" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1421,11 +1417,7 @@
       </c>
       <c r="E38" s="10" t="inlineStr"/>
       <c r="F38" s="10" t="inlineStr"/>
-      <c r="G38" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G38" s="10" t="inlineStr"/>
       <c r="H38" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1489,7 +1481,11 @@
           <t>31-January-2025</t>
         </is>
       </c>
-      <c r="C41" s="10" t="inlineStr"/>
+      <c r="C41" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D41" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1497,11 +1493,7 @@
       </c>
       <c r="E41" s="10" t="inlineStr"/>
       <c r="F41" s="10" t="inlineStr"/>
-      <c r="G41" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G41" s="10" t="inlineStr"/>
       <c r="H41" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1522,7 +1514,7 @@
       </c>
       <c r="C44" s="16" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="D44" s="16" t="inlineStr">
@@ -1532,17 +1524,17 @@
       </c>
       <c r="E44" s="16" t="inlineStr">
         <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="F44" s="16" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
-      <c r="F44" s="16" t="inlineStr">
-        <is>
-          <t>6.0</t>
-        </is>
-      </c>
       <c r="G44" s="16" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H44" s="14" t="n"/>

</xml_diff>

<commit_message>
added some sec changes
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -562,7 +562,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>GVT000ECI24000829</t>
+          <t>12345-ABC</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>PALO IT</t>
+          <t>adasdas dasd 66 Q</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>DevOps Engineer - II</t>
+          <t>DevOps Engineer</t>
         </is>
       </c>
     </row>
@@ -709,17 +709,17 @@
           <t>02-January-2025</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D12" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E12" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="E12" s="10" t="inlineStr"/>
       <c r="F12" s="10" t="inlineStr"/>
       <c r="G12" s="10" t="inlineStr"/>
       <c r="H12" s="13" t="inlineStr">
@@ -737,17 +737,17 @@
           <t>03-January-2025</t>
         </is>
       </c>
-      <c r="C13" s="10" t="inlineStr"/>
+      <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D13" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E13" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="E13" s="10" t="inlineStr"/>
       <c r="F13" s="10" t="inlineStr"/>
       <c r="G13" s="10" t="inlineStr"/>
       <c r="H13" s="13" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="C44" s="16" t="inlineStr">
         <is>
-          <t>18.0</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="D44" s="16" t="inlineStr">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="E44" s="16" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F44" s="16" t="inlineStr">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="B50" s="17" t="inlineStr">
         <is>
-          <t>07 - February - 2025</t>
+          <t>08 - February - 2025</t>
         </is>
       </c>
       <c r="H50" s="14" t="n"/>

</xml_diff>

<commit_message>
add more secured text feature
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -540,7 +540,7 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>To engage Agile Co-Development and ICT Professiona</t>
+          <t>To engage Agile Co-Development and ICT Professional Services via 19024 bulk tender (PR230941)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -709,7 +709,11 @@
           <t>02-January-2025</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr"/>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D12" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -717,11 +721,7 @@
       </c>
       <c r="E12" s="10" t="inlineStr"/>
       <c r="F12" s="10" t="inlineStr"/>
-      <c r="G12" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G12" s="10" t="inlineStr"/>
       <c r="H12" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -737,7 +737,11 @@
           <t>03-January-2025</t>
         </is>
       </c>
-      <c r="C13" s="10" t="inlineStr"/>
+      <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D13" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -745,11 +749,7 @@
       </c>
       <c r="E13" s="10" t="inlineStr"/>
       <c r="F13" s="10" t="inlineStr"/>
-      <c r="G13" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G13" s="10" t="inlineStr"/>
       <c r="H13" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1245,11 +1245,7 @@
           <t>22-January-2025</t>
         </is>
       </c>
-      <c r="C32" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C32" s="10" t="inlineStr"/>
       <c r="D32" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1257,7 +1253,11 @@
       </c>
       <c r="E32" s="10" t="inlineStr"/>
       <c r="F32" s="10" t="inlineStr"/>
-      <c r="G32" s="10" t="inlineStr"/>
+      <c r="G32" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H32" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1273,11 +1273,7 @@
           <t>23-January-2025</t>
         </is>
       </c>
-      <c r="C33" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C33" s="10" t="inlineStr"/>
       <c r="D33" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1285,7 +1281,11 @@
       </c>
       <c r="E33" s="10" t="inlineStr"/>
       <c r="F33" s="10" t="inlineStr"/>
-      <c r="G33" s="10" t="inlineStr"/>
+      <c r="G33" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H33" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1301,11 +1301,7 @@
           <t>24-January-2025</t>
         </is>
       </c>
-      <c r="C34" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C34" s="10" t="inlineStr"/>
       <c r="D34" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1313,7 +1309,11 @@
       </c>
       <c r="E34" s="10" t="inlineStr"/>
       <c r="F34" s="10" t="inlineStr"/>
-      <c r="G34" s="10" t="inlineStr"/>
+      <c r="G34" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H34" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1377,11 +1377,7 @@
           <t>27-January-2025</t>
         </is>
       </c>
-      <c r="C37" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C37" s="10" t="inlineStr"/>
       <c r="D37" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1389,7 +1385,11 @@
       </c>
       <c r="E37" s="10" t="inlineStr"/>
       <c r="F37" s="10" t="inlineStr"/>
-      <c r="G37" s="10" t="inlineStr"/>
+      <c r="G37" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H37" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1405,11 +1405,7 @@
           <t>28-January-2025</t>
         </is>
       </c>
-      <c r="C38" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C38" s="10" t="inlineStr"/>
       <c r="D38" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1417,7 +1413,11 @@
       </c>
       <c r="E38" s="10" t="inlineStr"/>
       <c r="F38" s="10" t="inlineStr"/>
-      <c r="G38" s="10" t="inlineStr"/>
+      <c r="G38" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H38" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1481,11 +1481,7 @@
           <t>31-January-2025</t>
         </is>
       </c>
-      <c r="C41" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C41" s="10" t="inlineStr"/>
       <c r="D41" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1493,7 +1489,11 @@
       </c>
       <c r="E41" s="10" t="inlineStr"/>
       <c r="F41" s="10" t="inlineStr"/>
-      <c r="G41" s="10" t="inlineStr"/>
+      <c r="G41" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H41" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="C44" s="16" t="inlineStr">
         <is>
-          <t>18.0</t>
+          <t>14.0</t>
         </is>
       </c>
       <c r="D44" s="16" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="G44" s="16" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="H44" s="14" t="n"/>

</xml_diff>

<commit_message>
Add reset user data feature
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -1245,7 +1245,11 @@
           <t>22-January-2025</t>
         </is>
       </c>
-      <c r="C32" s="10" t="inlineStr"/>
+      <c r="C32" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D32" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1253,11 +1257,7 @@
       </c>
       <c r="E32" s="10" t="inlineStr"/>
       <c r="F32" s="10" t="inlineStr"/>
-      <c r="G32" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G32" s="10" t="inlineStr"/>
       <c r="H32" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1273,7 +1273,11 @@
           <t>23-January-2025</t>
         </is>
       </c>
-      <c r="C33" s="10" t="inlineStr"/>
+      <c r="C33" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D33" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1281,11 +1285,7 @@
       </c>
       <c r="E33" s="10" t="inlineStr"/>
       <c r="F33" s="10" t="inlineStr"/>
-      <c r="G33" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G33" s="10" t="inlineStr"/>
       <c r="H33" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1301,7 +1301,11 @@
           <t>24-January-2025</t>
         </is>
       </c>
-      <c r="C34" s="10" t="inlineStr"/>
+      <c r="C34" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D34" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1309,11 +1313,7 @@
       </c>
       <c r="E34" s="10" t="inlineStr"/>
       <c r="F34" s="10" t="inlineStr"/>
-      <c r="G34" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G34" s="10" t="inlineStr"/>
       <c r="H34" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1377,7 +1377,11 @@
           <t>27-January-2025</t>
         </is>
       </c>
-      <c r="C37" s="10" t="inlineStr"/>
+      <c r="C37" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D37" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1385,11 +1389,7 @@
       </c>
       <c r="E37" s="10" t="inlineStr"/>
       <c r="F37" s="10" t="inlineStr"/>
-      <c r="G37" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G37" s="10" t="inlineStr"/>
       <c r="H37" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1405,7 +1405,11 @@
           <t>28-January-2025</t>
         </is>
       </c>
-      <c r="C38" s="10" t="inlineStr"/>
+      <c r="C38" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D38" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1413,11 +1417,7 @@
       </c>
       <c r="E38" s="10" t="inlineStr"/>
       <c r="F38" s="10" t="inlineStr"/>
-      <c r="G38" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G38" s="10" t="inlineStr"/>
       <c r="H38" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1481,7 +1481,11 @@
           <t>31-January-2025</t>
         </is>
       </c>
-      <c r="C41" s="10" t="inlineStr"/>
+      <c r="C41" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="D41" s="12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1489,11 +1493,7 @@
       </c>
       <c r="E41" s="10" t="inlineStr"/>
       <c r="F41" s="10" t="inlineStr"/>
-      <c r="G41" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="G41" s="10" t="inlineStr"/>
       <c r="H41" s="13" t="inlineStr">
         <is>
           <t>-</t>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="C44" s="16" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="D44" s="16" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="G44" s="16" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H44" s="14" t="n"/>

</xml_diff>

<commit_message>
docker file and other hcanges
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -600,7 +600,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>To engage Agile Co-Development ICT Professional Services via 19024 bulk tender (PR230941)</t>
+          <t>Agile Co-Development Services</t>
         </is>
       </c>
       <c r="C2" s="3" t="n"/>
@@ -626,7 +626,7 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>GVT000ECI24000829</t>
+          <t>GVT000ABC1234</t>
         </is>
       </c>
       <c r="C3" s="6" t="n"/>
@@ -704,7 +704,7 @@
       </c>
       <c r="B7" s="10" t="inlineStr">
         <is>
-          <t>DevOps Engineer - II</t>
+          <t>asdasdad</t>
         </is>
       </c>
       <c r="C7" s="11" t="n"/>
@@ -721,7 +721,7 @@
       </c>
       <c r="B8" s="10" t="inlineStr">
         <is>
-          <t>Consulting</t>
+          <t>asdasdConsulting</t>
         </is>
       </c>
       <c r="C8" s="11" t="n"/>
@@ -1294,9 +1294,7 @@
           <t>21-January-2025</t>
         </is>
       </c>
-      <c r="C31" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C31" s="21" t="inlineStr"/>
       <c r="D31" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1304,7 +1302,9 @@
       </c>
       <c r="E31" s="21" t="inlineStr"/>
       <c r="F31" s="21" t="inlineStr"/>
-      <c r="G31" s="21" t="inlineStr"/>
+      <c r="G31" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H31" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1320,9 +1320,7 @@
           <t>22-January-2025</t>
         </is>
       </c>
-      <c r="C32" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C32" s="21" t="inlineStr"/>
       <c r="D32" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1330,7 +1328,9 @@
       </c>
       <c r="E32" s="21" t="inlineStr"/>
       <c r="F32" s="21" t="inlineStr"/>
-      <c r="G32" s="21" t="inlineStr"/>
+      <c r="G32" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H32" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1346,9 +1346,7 @@
           <t>23-January-2025</t>
         </is>
       </c>
-      <c r="C33" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C33" s="21" t="inlineStr"/>
       <c r="D33" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1356,7 +1354,9 @@
       </c>
       <c r="E33" s="21" t="inlineStr"/>
       <c r="F33" s="21" t="inlineStr"/>
-      <c r="G33" s="21" t="inlineStr"/>
+      <c r="G33" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H33" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1372,9 +1372,7 @@
           <t>24-January-2025</t>
         </is>
       </c>
-      <c r="C34" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C34" s="21" t="inlineStr"/>
       <c r="D34" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1382,7 +1380,9 @@
       </c>
       <c r="E34" s="21" t="inlineStr"/>
       <c r="F34" s="21" t="inlineStr"/>
-      <c r="G34" s="21" t="inlineStr"/>
+      <c r="G34" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H34" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1446,9 +1446,7 @@
           <t>27-January-2025</t>
         </is>
       </c>
-      <c r="C37" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C37" s="21" t="inlineStr"/>
       <c r="D37" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1456,7 +1454,9 @@
       </c>
       <c r="E37" s="21" t="inlineStr"/>
       <c r="F37" s="21" t="inlineStr"/>
-      <c r="G37" s="21" t="inlineStr"/>
+      <c r="G37" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H37" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1472,9 +1472,7 @@
           <t>28-January-2025</t>
         </is>
       </c>
-      <c r="C38" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C38" s="21" t="inlineStr"/>
       <c r="D38" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1482,7 +1480,9 @@
       </c>
       <c r="E38" s="21" t="inlineStr"/>
       <c r="F38" s="21" t="inlineStr"/>
-      <c r="G38" s="21" t="inlineStr"/>
+      <c r="G38" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H38" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1542,9 +1542,7 @@
           <t>31-January-2025</t>
         </is>
       </c>
-      <c r="C41" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C41" s="21" t="inlineStr"/>
       <c r="D41" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1552,7 +1550,9 @@
       </c>
       <c r="E41" s="21" t="inlineStr"/>
       <c r="F41" s="21" t="inlineStr"/>
-      <c r="G41" s="21" t="inlineStr"/>
+      <c r="G41" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H41" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B44" s="5" t="n"/>
       <c r="C44" s="22" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D44" s="22" t="n">
         <v>3</v>
@@ -1600,10 +1600,8 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G44" s="22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="G44" s="22" t="n">
+        <v>7</v>
       </c>
       <c r="H44" s="26" t="n"/>
     </row>
@@ -1661,7 +1659,7 @@
       </c>
       <c r="B48" s="27" t="inlineStr">
         <is>
-          <t>11 - Feb - 2025</t>
+          <t>12 - Feb - 2025</t>
         </is>
       </c>
       <c r="C48" s="8" t="n"/>
@@ -1689,7 +1687,7 @@
       </c>
       <c r="B50" s="8" t="inlineStr">
         <is>
-          <t>Deepu Joseph</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C50" s="8" t="n"/>

</xml_diff>

<commit_message>
date overlap logic added
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -964,7 +964,9 @@
           <t>08-January-2025</t>
         </is>
       </c>
-      <c r="C18" s="21" t="inlineStr"/>
+      <c r="C18" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="D18" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -972,9 +974,7 @@
       </c>
       <c r="E18" s="21" t="inlineStr"/>
       <c r="F18" s="21" t="inlineStr"/>
-      <c r="G18" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G18" s="21" t="inlineStr"/>
       <c r="H18" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -990,7 +990,9 @@
           <t>09-January-2025</t>
         </is>
       </c>
-      <c r="C19" s="21" t="inlineStr"/>
+      <c r="C19" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="D19" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -998,9 +1000,7 @@
       </c>
       <c r="E19" s="21" t="inlineStr"/>
       <c r="F19" s="21" t="inlineStr"/>
-      <c r="G19" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G19" s="21" t="inlineStr"/>
       <c r="H19" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1016,7 +1016,9 @@
           <t>10-January-2025</t>
         </is>
       </c>
-      <c r="C20" s="21" t="inlineStr"/>
+      <c r="C20" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="D20" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1024,9 +1026,7 @@
       </c>
       <c r="E20" s="21" t="inlineStr"/>
       <c r="F20" s="21" t="inlineStr"/>
-      <c r="G20" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G20" s="21" t="inlineStr"/>
       <c r="H20" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1096,11 +1096,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E23" s="21" t="inlineStr"/>
+      <c r="E23" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="F23" s="21" t="inlineStr"/>
-      <c r="G23" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G23" s="21" t="inlineStr"/>
       <c r="H23" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1122,11 +1122,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E24" s="21" t="inlineStr"/>
+      <c r="E24" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="F24" s="21" t="inlineStr"/>
-      <c r="G24" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G24" s="21" t="inlineStr"/>
       <c r="H24" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1148,11 +1148,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E25" s="21" t="inlineStr"/>
+      <c r="E25" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="F25" s="21" t="inlineStr"/>
-      <c r="G25" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G25" s="21" t="inlineStr"/>
       <c r="H25" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1174,11 +1174,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E26" s="21" t="inlineStr"/>
+      <c r="E26" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="F26" s="21" t="inlineStr"/>
-      <c r="G26" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G26" s="21" t="inlineStr"/>
       <c r="H26" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1200,11 +1200,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E27" s="21" t="inlineStr"/>
+      <c r="E27" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="F27" s="21" t="inlineStr"/>
-      <c r="G27" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G27" s="21" t="inlineStr"/>
       <c r="H27" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1268,9 +1268,7 @@
           <t>20-January-2025</t>
         </is>
       </c>
-      <c r="C30" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C30" s="21" t="inlineStr"/>
       <c r="D30" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1278,7 +1276,9 @@
       </c>
       <c r="E30" s="21" t="inlineStr"/>
       <c r="F30" s="21" t="inlineStr"/>
-      <c r="G30" s="21" t="inlineStr"/>
+      <c r="G30" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H30" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1294,9 +1294,7 @@
           <t>21-January-2025</t>
         </is>
       </c>
-      <c r="C31" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C31" s="21" t="inlineStr"/>
       <c r="D31" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1304,7 +1302,9 @@
       </c>
       <c r="E31" s="21" t="inlineStr"/>
       <c r="F31" s="21" t="inlineStr"/>
-      <c r="G31" s="21" t="inlineStr"/>
+      <c r="G31" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H31" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1320,9 +1320,7 @@
           <t>22-January-2025</t>
         </is>
       </c>
-      <c r="C32" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C32" s="21" t="inlineStr"/>
       <c r="D32" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1330,7 +1328,9 @@
       </c>
       <c r="E32" s="21" t="inlineStr"/>
       <c r="F32" s="21" t="inlineStr"/>
-      <c r="G32" s="21" t="inlineStr"/>
+      <c r="G32" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H32" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1346,9 +1346,7 @@
           <t>23-January-2025</t>
         </is>
       </c>
-      <c r="C33" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C33" s="21" t="inlineStr"/>
       <c r="D33" s="22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1356,7 +1354,9 @@
       </c>
       <c r="E33" s="21" t="inlineStr"/>
       <c r="F33" s="21" t="inlineStr"/>
-      <c r="G33" s="21" t="inlineStr"/>
+      <c r="G33" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="H33" s="24" t="inlineStr">
         <is>
           <t>-</t>
@@ -1587,15 +1587,13 @@
       </c>
       <c r="B44" s="5" t="n"/>
       <c r="C44" s="22" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="E44" s="22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="E44" s="22" t="n">
+        <v>5</v>
       </c>
       <c r="F44" s="22" t="inlineStr">
         <is>
@@ -1603,7 +1601,7 @@
         </is>
       </c>
       <c r="G44" s="22" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H44" s="26" t="n"/>
     </row>

</xml_diff>